<commit_message>
Need to redact prediction in data generator
</commit_message>
<xml_diff>
--- a/Data for AI development.xlsx
+++ b/Data for AI development.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmasch\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAB\Kidney-Segmentation-Jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FE9B86-9C41-45DF-A116-C82423D7B4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28F4908-AFD9-4C72-9A23-6CC61C2F1EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="60" windowWidth="21705" windowHeight="14475" xr2:uid="{962D976F-899C-40B8-A93F-EAA9E9420A4F}"/>
+    <workbookView xWindow="6390" yWindow="2310" windowWidth="21600" windowHeight="12795" xr2:uid="{962D976F-899C-40B8-A93F-EAA9E9420A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -979,12 +979,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1021,10 +1020,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="15" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="16" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
@@ -1426,7 +1425,7 @@
   <dimension ref="B1:Y154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,11 +1433,9 @@
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="3.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" style="2" customWidth="1"/>
+    <col min="10" max="12" width="10.7109375" customWidth="1"/>
     <col min="13" max="13" width="3.7109375" customWidth="1"/>
     <col min="14" max="16" width="10.7109375" customWidth="1"/>
     <col min="18" max="18" width="17.42578125" customWidth="1"/>
@@ -1447,52 +1444,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="V1" s="28" t="s">
         <v>195</v>
       </c>
       <c r="W1" s="1"/>
-      <c r="X1" s="29" t="s">
+      <c r="X1" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="Y1" s="29" t="s">
+      <c r="Y1" s="28" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="2" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="F2" s="34" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="F2" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
-      <c r="J2" s="37" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
+      <c r="J2" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
-      <c r="N2" s="40" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="38"/>
+      <c r="N2" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42"/>
-      <c r="R2" s="29" t="s">
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
+      <c r="R2" s="28" t="s">
         <v>196</v>
       </c>
       <c r="S2" s="1">
@@ -1512,49 +1505,49 @@
         <f>SUM(S2:V2)</f>
         <v>151</v>
       </c>
-      <c r="Y2" s="33">
+      <c r="Y2" s="32">
         <f>X2/$X$6</f>
         <v>0.79894179894179895</v>
       </c>
     </row>
     <row r="3" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="N3" s="23" t="s">
+      <c r="N3" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="O3" s="23" t="s">
+      <c r="O3" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="P3" s="23" t="s">
+      <c r="P3" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="R3" s="29" t="s">
+      <c r="R3" s="28" t="s">
         <v>197</v>
       </c>
       <c r="S3" s="1">
@@ -1574,22 +1567,22 @@
         <f>SUM(S3:V3)</f>
         <v>19</v>
       </c>
-      <c r="Y3" s="33">
+      <c r="Y3" s="32">
         <f>X3/$X$6</f>
         <v>0.10052910052910052</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="29" t="s">
+      <c r="R4" s="28" t="s">
         <v>198</v>
       </c>
       <c r="S4" s="1">
@@ -1609,19 +1602,19 @@
         <f>SUM(S4:V4)</f>
         <v>19</v>
       </c>
-      <c r="Y4" s="33">
+      <c r="Y4" s="32">
         <f>X4/$X$6</f>
         <v>0.10052910052910052</v>
       </c>
     </row>
     <row r="5" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="S5" s="1"/>
@@ -1632,16 +1625,16 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="R6" s="29" t="s">
+      <c r="R6" s="28" t="s">
         <v>200</v>
       </c>
       <c r="S6" s="1">
@@ -1667,942 +1660,838 @@
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="13" t="s">
+    </row>
+    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="9" t="s">
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="s">
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="s">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="9" t="s">
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="9" t="s">
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="8" t="s">
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="8" t="s">
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="8" t="s">
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="8" t="s">
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="8" t="s">
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="8" t="s">
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="8" t="s">
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" s="8" t="s">
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B58" s="8" t="s">
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
-    </row>
-    <row r="59" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="10" t="s">
+    </row>
+    <row r="59" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-    </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B60" s="17" t="s">
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="18" t="s">
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B62" s="18" t="s">
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B63" s="18" t="s">
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B64" s="18" t="s">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="17" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="17" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="18" t="s">
+      <c r="B66" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="17" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="18" t="s">
+      <c r="B73" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="18" t="s">
+      <c r="B74" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="18" t="s">
+      <c r="B75" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="17" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="18" t="s">
+      <c r="B77" s="17" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="17" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="17" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="18" t="s">
+      <c r="B80" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="18" t="s">
+      <c r="B81" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="18" t="s">
+      <c r="B82" s="17" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="18" t="s">
+      <c r="B83" s="17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="18" t="s">
+      <c r="B84" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="17" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="18" t="s">
+      <c r="B89" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="18" t="s">
+      <c r="B90" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="18" t="s">
+      <c r="B92" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="18" t="s">
+      <c r="B94" s="17" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="18" t="s">
+      <c r="B95" s="17" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="96" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="19" t="s">
+      <c r="B96" s="18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="25" t="s">
+      <c r="B97" s="24" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="26" t="s">
+      <c r="B98" s="25" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="26" t="s">
+      <c r="B99" s="25" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="26" t="s">
+      <c r="B100" s="25" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="26" t="s">
+      <c r="B101" s="25" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="27" t="s">
+      <c r="B102" s="26" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="27" t="s">
+      <c r="B103" s="26" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="26" t="s">
+      <c r="B104" s="25" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="26" t="s">
+      <c r="B105" s="25" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="26" t="s">
+      <c r="B106" s="25" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="26" t="s">
+      <c r="B107" s="25" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="26" t="s">
+      <c r="B108" s="25" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="26" t="s">
+      <c r="B109" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="26" t="s">
+      <c r="B110" s="25" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="26" t="s">
+      <c r="B111" s="25" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="26" t="s">
+      <c r="B112" s="25" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="26" t="s">
+      <c r="B113" s="25" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="26" t="s">
+      <c r="B114" s="25" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="26" t="s">
+      <c r="B115" s="25" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="26" t="s">
+      <c r="B116" s="25" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="26" t="s">
+      <c r="B117" s="25" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="26" t="s">
+      <c r="B118" s="25" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="26" t="s">
+      <c r="B119" s="25" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="26" t="s">
+      <c r="B120" s="25" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="26" t="s">
+      <c r="B121" s="25" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="26" t="s">
+      <c r="B122" s="25" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="26" t="s">
+      <c r="B123" s="25" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="26" t="s">
+      <c r="B124" s="25" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="26" t="s">
+      <c r="B125" s="25" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="26" t="s">
+      <c r="B126" s="25" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="26" t="s">
+      <c r="B127" s="25" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="26" t="s">
+      <c r="B128" s="25" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="26" t="s">
+      <c r="B129" s="25" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="26" t="s">
+      <c r="B130" s="25" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="26" t="s">
+      <c r="B131" s="25" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="26" t="s">
+      <c r="B132" s="25" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="26" t="s">
+      <c r="B133" s="25" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="26" t="s">
+      <c r="B134" s="25" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="26" t="s">
+      <c r="B135" s="25" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="26" t="s">
+      <c r="B136" s="25" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="26" t="s">
+      <c r="B137" s="25" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="26" t="s">
+      <c r="B138" s="25" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="26" t="s">
+      <c r="B139" s="25" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="26" t="s">
+      <c r="B140" s="25" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="26" t="s">
+      <c r="B141" s="25" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="26" t="s">
+      <c r="B142" s="25" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="26" t="s">
+      <c r="B143" s="25" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="26" t="s">
+      <c r="B144" s="25" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="26" t="s">
+      <c r="B145" s="25" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="26" t="s">
+      <c r="B146" s="25" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="26" t="s">
+      <c r="B147" s="25" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="26" t="s">
+      <c r="B148" s="25" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="26" t="s">
+      <c r="B149" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="26" t="s">
+      <c r="B150" s="25" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="26" t="s">
+      <c r="B151" s="25" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="26" t="s">
+      <c r="B152" s="25" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="26" t="s">
+      <c r="B153" s="25" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="154" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="28" t="s">
+      <c r="B154" s="27" t="s">
         <v>188</v>
       </c>
     </row>

</xml_diff>